<commit_message>
creating tables and excel file for investigating messy HUCs
</commit_message>
<xml_diff>
--- a/docs/location_tables_99999999_HUCs.xlsx
+++ b/docs/location_tables_99999999_HUCs.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rory/Desktop/Grad School/Capstone - ESA Listed Fish Species/ESA_Permits_Capstone/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D95BF3E-2D6F-C345-819F-740B7228A554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{367DEA83-4886-5947-B904-59172091920E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32600" yWindow="-2860" windowWidth="28220" windowHeight="17500"/>
   </bookViews>
   <sheets>
-    <sheet name="Adults Table" sheetId="1" r:id="rId1"/>
-    <sheet name="Juveniles Table" sheetId="2" r:id="rId2"/>
+    <sheet name="README" sheetId="3" r:id="rId1"/>
+    <sheet name="Adults Table" sheetId="1" r:id="rId2"/>
+    <sheet name="Juveniles Table" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>California inland estuarine, delta, and freshwaters</t>
   </si>
@@ -186,6 +187,9 @@
   </si>
   <si>
     <t>Willamette, Middle Fork Willamette, Coast Fork Willamette, Calapooia, Long Tom, Marys and Luckiamute Rivers</t>
+  </si>
+  <si>
+    <t>Tables display counts of the fields "WaterbodyName" and "StreamName" for those permits with HUC codes of '99999999'. The rows of the table come from "WaterbodyName" and the columns come from "StreamName". ***Note that there are some permits with HUCs labeled as "NA", although there were far fewer and they all come from the same permit (and thus are not included in the tables presented here). The location description on that permit is for "all waterbodies in the Puget Sound...", while the WaterbodyName was "Admiralty Inlet".</t>
   </si>
 </sst>
 </file>
@@ -688,7 +692,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -701,6 +705,9 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1056,10 +1063,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:K20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:K20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1470,12 +1701,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AW15"/>
   <sheetViews>
-    <sheetView topLeftCell="X4" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>